<commit_message>
Updated glossary and index
</commit_message>
<xml_diff>
--- a/DWV_Index/Glossary_WOTUS2020_DWV_Index.xlsx
+++ b/DWV_Index/Glossary_WOTUS2020_DWV_Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamali/NMStory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CFD411-1398-3D4F-B292-9221082C376E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8740C7D6-5E91-FB4F-B8F6-88A6EA3E46C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2820" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="2840" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary_WOTUS2020_DWV_Index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Variable</t>
   </si>
@@ -34,155 +34,329 @@
     <t>Main City</t>
   </si>
   <si>
-    <t>Main Water Type</t>
-  </si>
-  <si>
-    <t>NUMBER0</t>
-  </si>
-  <si>
-    <t>SYSTEM NAME</t>
-  </si>
-  <si>
-    <t>PWS Type</t>
-  </si>
-  <si>
-    <t>D_TOT_POPULATION</t>
-  </si>
-  <si>
-    <t>D_TTL_STOR</t>
-  </si>
-  <si>
     <t>total_intakes</t>
   </si>
   <si>
-    <t>Total Num. of  GW, GU or SW intakes</t>
-  </si>
-  <si>
     <t>total_gu_sw_intakes</t>
   </si>
   <si>
-    <t>Total Num. of GU or SW  intakes</t>
-  </si>
-  <si>
     <t>gu_intakes</t>
   </si>
   <si>
-    <t>Num. of GU Intakes</t>
-  </si>
-  <si>
     <t>gw_intakes</t>
   </si>
   <si>
-    <t>Num. of GW  Intakes</t>
-  </si>
-  <si>
     <t>sw_intakes</t>
   </si>
   <si>
-    <t>Num. of SW Intakes</t>
-  </si>
-  <si>
     <t>impacted_gu_sw_water_intakes</t>
   </si>
   <si>
-    <t>Num. of GU or SW Water Intakes Impacted</t>
-  </si>
-  <si>
     <t>impacted_gu_intakes</t>
   </si>
   <si>
-    <t>Num. of Impacted GU Intakes</t>
-  </si>
-  <si>
     <t>impacted_sw_intakes</t>
   </si>
   <si>
-    <t>Num. of Impacted SW Intakes</t>
-  </si>
-  <si>
     <t>ratio_impacted_gu_sw_over_all</t>
   </si>
   <si>
-    <t>Num. of GU or SW intakes impacted over Total Num of GW, GU or SW intakes</t>
-  </si>
-  <si>
     <t>ratio_gu_sw_impacted_over_gu_sw</t>
   </si>
   <si>
-    <t>Num. of GU or SW intakes impacted over Total num. of GU or SW water Intakes</t>
-  </si>
-  <si>
-    <t>sizetypeid</t>
-  </si>
-  <si>
-    <t>Size Type ID</t>
-  </si>
-  <si>
-    <t>sizetype</t>
-  </si>
-  <si>
-    <t>mhipws</t>
-  </si>
-  <si>
-    <t>MHI PWS</t>
-  </si>
-  <si>
     <t>ratio_pws_mhi_over_state_mhi</t>
   </si>
   <si>
-    <t>Ratio PWS MHI/State MHI ($48,059)</t>
-  </si>
-  <si>
     <t>disadvantage_status_type</t>
   </si>
   <si>
-    <t>Severely Disadvantage Community (PWS MHI 80% or less State MHI); Disadvantaged Community (PWS MHI 100% or less State MHI); Non Disadvanteged Community (PWS MHI Above State MHI)</t>
-  </si>
-  <si>
-    <t>cws_impacted</t>
-  </si>
-  <si>
-    <t>alternative_water_type</t>
-  </si>
-  <si>
-    <t>small_system_pop_10000_less</t>
-  </si>
-  <si>
     <t>wotus2020_dwv_index</t>
   </si>
   <si>
-    <t>CWS Impacted</t>
-  </si>
-  <si>
-    <t>Has water intakes with water type different from SW or GU.</t>
-  </si>
-  <si>
-    <t>Small system (Population 10,000 or less)</t>
-  </si>
-  <si>
-    <t>Size Type</t>
-  </si>
-  <si>
-    <t>D_PRIN_CNT</t>
-  </si>
-  <si>
-    <t>D_PRIN_CIT</t>
-  </si>
-  <si>
-    <t>D_FED_PRIM</t>
-  </si>
-  <si>
-    <t>WOTUS 2020 Drinking Water Vulnerability Index</t>
-  </si>
-  <si>
-    <t>PWS_TYPE</t>
+    <t>number0</t>
+  </si>
+  <si>
+    <t>system_nam</t>
+  </si>
+  <si>
+    <t>owner_type</t>
+  </si>
+  <si>
+    <t>d_prin_cit</t>
+  </si>
+  <si>
+    <t>d_prin_cnt</t>
+  </si>
+  <si>
+    <t>d_fed_prim</t>
+  </si>
+  <si>
+    <t>d_populati</t>
+  </si>
+  <si>
+    <t>d_ttl_stor</t>
+  </si>
+  <si>
+    <t>d_pws_fed_</t>
+  </si>
+  <si>
+    <t>has_nmdwb_data</t>
+  </si>
+  <si>
+    <t>num_gw_facilities</t>
+  </si>
+  <si>
+    <t>has_gw_facilities_ind</t>
+  </si>
+  <si>
+    <t>num_sw_gu_facilities</t>
+  </si>
+  <si>
+    <t>num_sw_facilities</t>
+  </si>
+  <si>
+    <t>num_gu_facilities</t>
+  </si>
+  <si>
+    <t>has_sw_facilities_ind</t>
+  </si>
+  <si>
+    <t>has_gu_facilities_ind</t>
+  </si>
+  <si>
+    <t>surface_ground_facility_type</t>
+  </si>
+  <si>
+    <t>surf_wtr_ratio_if_spws</t>
+  </si>
+  <si>
+    <t>surf_wtr_pur_ratio_if_spws</t>
+  </si>
+  <si>
+    <t>grnd_wtr_udi_ratio_if_spws</t>
+  </si>
+  <si>
+    <t>grnd_wtr_udi_purch_if_spws</t>
+  </si>
+  <si>
+    <t>surface_pws</t>
+  </si>
+  <si>
+    <t>surface_ratio_if_spws</t>
+  </si>
+  <si>
+    <t>has_source_ratio_surface_pws</t>
+  </si>
+  <si>
+    <t>mhi_2010</t>
+  </si>
+  <si>
+    <t>has_mhi_data</t>
+  </si>
+  <si>
+    <t>has_drinking_water_data</t>
+  </si>
+  <si>
+    <t>alternative_intakes</t>
+  </si>
+  <si>
+    <t>has_surface_intake_geo_info</t>
+  </si>
+  <si>
+    <t>seller_number0_1</t>
+  </si>
+  <si>
+    <t>seller_system_name_1</t>
+  </si>
+  <si>
+    <t>seller_pop_1</t>
+  </si>
+  <si>
+    <t>seller_number0_2</t>
+  </si>
+  <si>
+    <t>seller_system_name_2</t>
+  </si>
+  <si>
+    <t>seller_pop_2</t>
+  </si>
+  <si>
+    <t>surfacepurchaser_status</t>
+  </si>
+  <si>
+    <t>has_surfacepurchase_data</t>
+  </si>
+  <si>
+    <t>seller_wotus2020_dwv_index_1</t>
+  </si>
+  <si>
+    <t>seller_wotus2020_dwv_index_2</t>
+  </si>
+  <si>
+    <t>index_summary</t>
+  </si>
+  <si>
+    <t>indicator if the pws active water intakes</t>
+  </si>
+  <si>
+    <t>Number of active ground water facilities</t>
+  </si>
+  <si>
+    <t>Indicator if the pws active ground water facilities</t>
+  </si>
+  <si>
+    <t>Id for the System</t>
+  </si>
+  <si>
+    <t>Water system Name</t>
+  </si>
+  <si>
+    <t>Owner Type</t>
+  </si>
+  <si>
+    <t>Primary Water Source</t>
+  </si>
+  <si>
+    <t>Population Served</t>
+  </si>
+  <si>
+    <t>TTL Stor</t>
+  </si>
+  <si>
+    <t>Main water source</t>
+  </si>
+  <si>
+    <t>Number of active SW facilities</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has active SW facilities</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has active GU facilities</t>
+  </si>
+  <si>
+    <t>{Surface, Ground or Surface and Ground}</t>
+  </si>
+  <si>
+    <t>Surface Water - Purchase Ratio (Only available for SW or GU PWS)</t>
+  </si>
+  <si>
+    <t>SW Ratio (Only available for SW or GU PWS)</t>
+  </si>
+  <si>
+    <t>GU  Ratio (Only available for SW or GU PWS)</t>
+  </si>
+  <si>
+    <t>GU - Purchase Ratio (Only available for SW or GU PWS)</t>
+  </si>
+  <si>
+    <t>Indicator if SW or GU PWS</t>
+  </si>
+  <si>
+    <t>PWS's Seller of Surface Purchase Water ID (1)</t>
+  </si>
+  <si>
+    <t>PWS's Seller of Surface Purchase Water System Name (1)</t>
+  </si>
+  <si>
+    <t>Seller Population (1)</t>
+  </si>
+  <si>
+    <t>PWS's Seller of Surface Purchase Water ID (2)</t>
+  </si>
+  <si>
+    <t>PWS's Seller of Surface Purchase Water System Name (2)</t>
+  </si>
+  <si>
+    <t>Seller Population (2)</t>
+  </si>
+  <si>
+    <t>Active  Surface Water Purchaser?</t>
+  </si>
+  <si>
+    <t>Has Surface Water Purchaser Data</t>
+  </si>
+  <si>
+    <t>Index Summary</t>
+  </si>
+  <si>
+    <t>SW, GU ratio to all water consumption</t>
+  </si>
+  <si>
+    <t>PWS has data on surface water ratios</t>
+  </si>
+  <si>
+    <t>PWS has data on MHI</t>
+  </si>
+  <si>
+    <t>PWS has data on active drinking water intake</t>
+  </si>
+  <si>
+    <t>Ratio of PWS's MHI over State's MHI</t>
+  </si>
+  <si>
+    <t>Disadvantage Community Status</t>
+  </si>
+  <si>
+    <t>PWS's Total active intakes</t>
+  </si>
+  <si>
+    <t>PWS's Total active surface water intakes</t>
+  </si>
+  <si>
+    <t>PWS's Total active ground water intakes</t>
+  </si>
+  <si>
+    <t>PWS's Total GU and SW intakes</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has non GU or SW intakes</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has any SW intake within .5 miles of an unprotected stream</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has any GU intake within .5 miles of an unprotected stream</t>
+  </si>
+  <si>
+    <t>Indicator if the PWS has any SW or GU intake within .5 miles of an unprotected stream</t>
+  </si>
+  <si>
+    <t>Number of impacted GU and SW intakes over total number of intakes</t>
+  </si>
+  <si>
+    <t>Number of impacted GU and SW intakes over GU and SW intakes</t>
+  </si>
+  <si>
+    <t>Indicator if PWS has active drinking water intakes</t>
+  </si>
+  <si>
+    <t>Number of active surface water (SW) or ground water under the direct influence of surface water (GU) facilities</t>
+  </si>
+  <si>
+    <t>Number of GU facilities</t>
+  </si>
+  <si>
+    <t>PWS's total active GU intakes</t>
+  </si>
+  <si>
+    <t>Seller 1's WOTUS 2020 Drinking Water Vulnerability Index</t>
+  </si>
+  <si>
+    <t>Seller 2's WOTUS 2020 Drinking Water Vulnerability Index</t>
+  </si>
+  <si>
+    <t>Median household income (MHI) 2010 (metric authored for challenge)</t>
+  </si>
+  <si>
+    <t>WOTUS 2020 Drinking Water Vulnerability Index (index authored for challenge)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,6 +487,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,9 +840,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1017,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,31 +1221,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1071,186 +1253,402 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>